<commit_message>
New version of industry_aggregations.xlsx file.
</commit_message>
<xml_diff>
--- a/inst/aggregation_tables/industry_aggregations.xlsx
+++ b/inst/aggregation_tables/industry_aggregations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/CLPFUDecompositionDatabase/inst/aggregation_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0693BB29-8AFC-BD4A-9ACA-5B38AB9604BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E185EE-74A3-F247-98C3-97A1DC310C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{6196F350-644F-294F-9730-D810A8B27C87}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>